<commit_message>
Updated script for data analysis
</commit_message>
<xml_diff>
--- a/data/anonymized/anonymized_data.xlsx
+++ b/data/anonymized/anonymized_data.xlsx
@@ -1,139 +1,146 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <workbookPr date1904="false"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b31428c643243b54/Dokumenter/ITU/fifth_semester/SecurityAndPrivacy/SecPriv-final-project/data/anonymized/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="4" documentId="11_EE72312E1DE1689DCE06394E5F7A0E65625CDAA2" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{34E525A1-5542-4153-BF27-87F8C9A718DA}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11836" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1391" uniqueCount="38">
   <si>
-    <t xml:space="preserve">m_sex</t>
+    <t>m_sex</t>
   </si>
   <si>
-    <t xml:space="preserve">m_evote</t>
+    <t>m_evote</t>
   </si>
   <si>
-    <t xml:space="preserve">m_dob</t>
+    <t>m_dob</t>
   </si>
   <si>
-    <t xml:space="preserve">m_zip</t>
+    <t>m_zip</t>
   </si>
   <si>
-    <t xml:space="preserve">education</t>
+    <t>education</t>
   </si>
   <si>
-    <t xml:space="preserve">m_citizenship_region</t>
+    <t>m_citizenship_region</t>
   </si>
   <si>
-    <t xml:space="preserve">m_marital_status</t>
+    <t>m_marital_status</t>
   </si>
   <si>
-    <t xml:space="preserve">m_party</t>
+    <t>m_party</t>
   </si>
   <si>
-    <t xml:space="preserve">Female</t>
+    <t>Female</t>
   </si>
   <si>
-    <t xml:space="preserve">&gt;=2000s</t>
+    <t>&gt;=2000s</t>
   </si>
   <si>
-    <t xml:space="preserve">2100</t>
+    <t>2100</t>
   </si>
   <si>
-    <t xml:space="preserve">Upper secondary education</t>
+    <t>Upper secondary education</t>
   </si>
   <si>
-    <t xml:space="preserve">Denmark</t>
+    <t>Denmark</t>
   </si>
   <si>
-    <t xml:space="preserve">Divorced</t>
+    <t>Divorced</t>
   </si>
   <si>
-    <t xml:space="preserve">Green</t>
+    <t>Green</t>
   </si>
   <si>
-    <t xml:space="preserve">1990s</t>
+    <t>1990s</t>
   </si>
   <si>
-    <t xml:space="preserve">2400</t>
+    <t>2400</t>
   </si>
   <si>
-    <t xml:space="preserve">Married/separated</t>
+    <t>Married/separated</t>
   </si>
   <si>
-    <t xml:space="preserve">Red</t>
+    <t>Red</t>
   </si>
   <si>
-    <t xml:space="preserve">1980s</t>
+    <t>1980s</t>
   </si>
   <si>
-    <t xml:space="preserve">2200</t>
+    <t>2200</t>
   </si>
   <si>
-    <t xml:space="preserve">Vocational bachelors educations</t>
+    <t>Vocational bachelors educations</t>
   </si>
   <si>
-    <t xml:space="preserve">Primary education</t>
+    <t>Primary education</t>
   </si>
   <si>
-    <t xml:space="preserve">1970s</t>
+    <t>1970s</t>
   </si>
   <si>
-    <t xml:space="preserve">Vocational Education and Training (VET)</t>
+    <t>Vocational Education and Training (VET)</t>
   </si>
   <si>
-    <t xml:space="preserve">Never married</t>
+    <t>Never married</t>
   </si>
   <si>
-    <t xml:space="preserve">Masters programmes</t>
+    <t>Masters programmes</t>
   </si>
   <si>
-    <t xml:space="preserve">Other</t>
+    <t>Other</t>
   </si>
   <si>
-    <t xml:space="preserve">Male</t>
+    <t>Male</t>
   </si>
   <si>
-    <t xml:space="preserve">2300</t>
+    <t>2300</t>
   </si>
   <si>
-    <t xml:space="preserve">1950s</t>
+    <t>1950s</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;=1940s</t>
+    <t>&lt;=1940s</t>
   </si>
   <si>
-    <t xml:space="preserve">1960s</t>
+    <t>1960s</t>
   </si>
   <si>
-    <t xml:space="preserve">Widowed</t>
+    <t>Widowed</t>
   </si>
   <si>
-    <t xml:space="preserve">Short cycle higher education</t>
+    <t>Short cycle higher education</t>
   </si>
   <si>
-    <t xml:space="preserve">Not stated</t>
+    <t>Not stated</t>
   </si>
   <si>
-    <t xml:space="preserve">Bachelors programmes</t>
+    <t>Bachelors programmes</t>
   </si>
   <si>
-    <t xml:space="preserve">Invalid vote</t>
+    <t>Invalid vote</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -169,6 +176,15 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -450,14 +466,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H201"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="true"/>
+    <sheetView tabSelected="1" topLeftCell="A178" workbookViewId="0">
+      <selection sqref="A1:H201"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -483,11 +501,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" t="n">
+      <c r="B2">
         <v>0</v>
       </c>
       <c r="C2" t="s">
@@ -509,11 +527,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="n">
+      <c r="B3">
         <v>1</v>
       </c>
       <c r="C3" t="s">
@@ -535,11 +553,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" t="n">
+      <c r="B4">
         <v>0</v>
       </c>
       <c r="C4" t="s">
@@ -561,11 +579,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>8</v>
       </c>
-      <c r="B5" t="n">
+      <c r="B5">
         <v>0</v>
       </c>
       <c r="C5" t="s">
@@ -587,11 +605,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>8</v>
       </c>
-      <c r="B6" t="n">
+      <c r="B6">
         <v>0</v>
       </c>
       <c r="C6" t="s">
@@ -613,11 +631,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>8</v>
       </c>
-      <c r="B7" t="n">
+      <c r="B7">
         <v>1</v>
       </c>
       <c r="C7" t="s">
@@ -639,17 +657,16 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>8</v>
       </c>
-      <c r="B8" t="n">
+      <c r="B8">
         <v>1</v>
       </c>
       <c r="C8" t="s">
         <v>19</v>
       </c>
-      <c r="D8"/>
       <c r="E8" t="s">
         <v>26</v>
       </c>
@@ -663,11 +680,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>28</v>
       </c>
-      <c r="B9" t="n">
+      <c r="B9">
         <v>0</v>
       </c>
       <c r="C9" t="s">
@@ -689,11 +706,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>28</v>
       </c>
-      <c r="B10" t="n">
+      <c r="B10">
         <v>1</v>
       </c>
       <c r="C10" t="s">
@@ -715,11 +732,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>28</v>
       </c>
-      <c r="B11" t="n">
+      <c r="B11">
         <v>1</v>
       </c>
       <c r="C11" t="s">
@@ -741,17 +758,16 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>28</v>
       </c>
-      <c r="B12" t="n">
+      <c r="B12">
         <v>0</v>
       </c>
       <c r="C12" t="s">
         <v>30</v>
       </c>
-      <c r="D12"/>
       <c r="E12" t="s">
         <v>22</v>
       </c>
@@ -765,11 +781,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>28</v>
       </c>
-      <c r="B13" t="n">
+      <c r="B13">
         <v>1</v>
       </c>
       <c r="C13" t="s">
@@ -791,11 +807,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>28</v>
       </c>
-      <c r="B14" t="n">
+      <c r="B14">
         <v>0</v>
       </c>
       <c r="C14" t="s">
@@ -817,11 +833,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>8</v>
       </c>
-      <c r="B15" t="n">
+      <c r="B15">
         <v>1</v>
       </c>
       <c r="C15" t="s">
@@ -843,11 +859,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>8</v>
       </c>
-      <c r="B16" t="n">
+      <c r="B16">
         <v>1</v>
       </c>
       <c r="C16" t="s">
@@ -869,11 +885,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>28</v>
       </c>
-      <c r="B17" t="n">
+      <c r="B17">
         <v>0</v>
       </c>
       <c r="C17" t="s">
@@ -895,11 +911,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>28</v>
       </c>
-      <c r="B18" t="n">
+      <c r="B18">
         <v>0</v>
       </c>
       <c r="C18" t="s">
@@ -921,11 +937,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>8</v>
       </c>
-      <c r="B19" t="n">
+      <c r="B19">
         <v>1</v>
       </c>
       <c r="C19" t="s">
@@ -947,11 +963,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>8</v>
       </c>
-      <c r="B20" t="n">
+      <c r="B20">
         <v>1</v>
       </c>
       <c r="C20" t="s">
@@ -973,11 +989,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>28</v>
       </c>
-      <c r="B21" t="n">
+      <c r="B21">
         <v>1</v>
       </c>
       <c r="C21" t="s">
@@ -999,11 +1015,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>8</v>
       </c>
-      <c r="B22" t="n">
+      <c r="B22">
         <v>0</v>
       </c>
       <c r="C22" t="s">
@@ -1025,11 +1041,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>28</v>
       </c>
-      <c r="B23" t="n">
+      <c r="B23">
         <v>1</v>
       </c>
       <c r="C23" t="s">
@@ -1051,11 +1067,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>8</v>
       </c>
-      <c r="B24" t="n">
+      <c r="B24">
         <v>0</v>
       </c>
       <c r="C24" t="s">
@@ -1077,11 +1093,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>28</v>
       </c>
-      <c r="B25" t="n">
+      <c r="B25">
         <v>0</v>
       </c>
       <c r="C25" t="s">
@@ -1103,11 +1119,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>28</v>
       </c>
-      <c r="B26" t="n">
+      <c r="B26">
         <v>1</v>
       </c>
       <c r="C26" t="s">
@@ -1129,11 +1145,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>28</v>
       </c>
-      <c r="B27" t="n">
+      <c r="B27">
         <v>1</v>
       </c>
       <c r="C27" t="s">
@@ -1155,11 +1171,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>28</v>
       </c>
-      <c r="B28" t="n">
+      <c r="B28">
         <v>0</v>
       </c>
       <c r="C28" t="s">
@@ -1181,11 +1197,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>8</v>
       </c>
-      <c r="B29" t="n">
+      <c r="B29">
         <v>1</v>
       </c>
       <c r="C29" t="s">
@@ -1207,11 +1223,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>8</v>
       </c>
-      <c r="B30" t="n">
+      <c r="B30">
         <v>1</v>
       </c>
       <c r="C30" t="s">
@@ -1233,11 +1249,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>28</v>
       </c>
-      <c r="B31" t="n">
+      <c r="B31">
         <v>1</v>
       </c>
       <c r="C31" t="s">
@@ -1259,17 +1275,16 @@
         <v>18</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>28</v>
       </c>
-      <c r="B32" t="n">
+      <c r="B32">
         <v>1</v>
       </c>
       <c r="C32" t="s">
         <v>30</v>
       </c>
-      <c r="D32"/>
       <c r="E32" t="s">
         <v>22</v>
       </c>
@@ -1283,11 +1298,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>28</v>
       </c>
-      <c r="B33" t="n">
+      <c r="B33">
         <v>0</v>
       </c>
       <c r="C33" t="s">
@@ -1309,11 +1324,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>8</v>
       </c>
-      <c r="B34" t="n">
+      <c r="B34">
         <v>0</v>
       </c>
       <c r="C34" t="s">
@@ -1335,17 +1350,16 @@
         <v>18</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>8</v>
       </c>
-      <c r="B35" t="n">
+      <c r="B35">
         <v>1</v>
       </c>
       <c r="C35" t="s">
         <v>19</v>
       </c>
-      <c r="D35"/>
       <c r="E35" t="s">
         <v>34</v>
       </c>
@@ -1359,11 +1373,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>28</v>
       </c>
-      <c r="B36" t="n">
+      <c r="B36">
         <v>0</v>
       </c>
       <c r="C36" t="s">
@@ -1385,11 +1399,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>8</v>
       </c>
-      <c r="B37" t="n">
+      <c r="B37">
         <v>1</v>
       </c>
       <c r="C37" t="s">
@@ -1411,11 +1425,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
         <v>28</v>
       </c>
-      <c r="B38" t="n">
+      <c r="B38">
         <v>1</v>
       </c>
       <c r="C38" t="s">
@@ -1437,11 +1451,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>8</v>
       </c>
-      <c r="B39" t="n">
+      <c r="B39">
         <v>0</v>
       </c>
       <c r="C39" t="s">
@@ -1463,11 +1477,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
         <v>8</v>
       </c>
-      <c r="B40" t="n">
+      <c r="B40">
         <v>0</v>
       </c>
       <c r="C40" t="s">
@@ -1489,11 +1503,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
         <v>28</v>
       </c>
-      <c r="B41" t="n">
+      <c r="B41">
         <v>1</v>
       </c>
       <c r="C41" t="s">
@@ -1515,11 +1529,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="42">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
         <v>28</v>
       </c>
-      <c r="B42" t="n">
+      <c r="B42">
         <v>0</v>
       </c>
       <c r="C42" t="s">
@@ -1541,11 +1555,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="43">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
         <v>28</v>
       </c>
-      <c r="B43" t="n">
+      <c r="B43">
         <v>0</v>
       </c>
       <c r="C43" t="s">
@@ -1567,11 +1581,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="44">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
         <v>28</v>
       </c>
-      <c r="B44" t="n">
+      <c r="B44">
         <v>1</v>
       </c>
       <c r="C44" t="s">
@@ -1593,11 +1607,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="45">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
         <v>8</v>
       </c>
-      <c r="B45" t="n">
+      <c r="B45">
         <v>0</v>
       </c>
       <c r="C45" t="s">
@@ -1619,11 +1633,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="46">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
         <v>28</v>
       </c>
-      <c r="B46" t="n">
+      <c r="B46">
         <v>0</v>
       </c>
       <c r="C46" t="s">
@@ -1645,11 +1659,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="47">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
         <v>28</v>
       </c>
-      <c r="B47" t="n">
+      <c r="B47">
         <v>0</v>
       </c>
       <c r="C47" t="s">
@@ -1671,11 +1685,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="48">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
         <v>28</v>
       </c>
-      <c r="B48" t="n">
+      <c r="B48">
         <v>0</v>
       </c>
       <c r="C48" t="s">
@@ -1697,11 +1711,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="49">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
         <v>8</v>
       </c>
-      <c r="B49" t="n">
+      <c r="B49">
         <v>1</v>
       </c>
       <c r="C49" t="s">
@@ -1723,11 +1737,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="50">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
         <v>28</v>
       </c>
-      <c r="B50" t="n">
+      <c r="B50">
         <v>1</v>
       </c>
       <c r="C50" t="s">
@@ -1749,11 +1763,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="51">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
         <v>28</v>
       </c>
-      <c r="B51" t="n">
+      <c r="B51">
         <v>1</v>
       </c>
       <c r="C51" t="s">
@@ -1775,11 +1789,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="52">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
         <v>8</v>
       </c>
-      <c r="B52" t="n">
+      <c r="B52">
         <v>0</v>
       </c>
       <c r="C52" t="s">
@@ -1801,11 +1815,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="53">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
         <v>8</v>
       </c>
-      <c r="B53" t="n">
+      <c r="B53">
         <v>0</v>
       </c>
       <c r="C53" t="s">
@@ -1827,11 +1841,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="54">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
         <v>8</v>
       </c>
-      <c r="B54" t="n">
+      <c r="B54">
         <v>0</v>
       </c>
       <c r="C54" t="s">
@@ -1853,11 +1867,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="55">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
         <v>28</v>
       </c>
-      <c r="B55" t="n">
+      <c r="B55">
         <v>1</v>
       </c>
       <c r="C55" t="s">
@@ -1879,11 +1893,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="56">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
         <v>28</v>
       </c>
-      <c r="B56" t="n">
+      <c r="B56">
         <v>1</v>
       </c>
       <c r="C56" t="s">
@@ -1905,11 +1919,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="57">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
         <v>8</v>
       </c>
-      <c r="B57" t="n">
+      <c r="B57">
         <v>0</v>
       </c>
       <c r="C57" t="s">
@@ -1931,11 +1945,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="58">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
         <v>8</v>
       </c>
-      <c r="B58" t="n">
+      <c r="B58">
         <v>0</v>
       </c>
       <c r="C58" t="s">
@@ -1957,11 +1971,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="59">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
         <v>8</v>
       </c>
-      <c r="B59" t="n">
+      <c r="B59">
         <v>0</v>
       </c>
       <c r="C59" t="s">
@@ -1983,11 +1997,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="60">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
         <v>28</v>
       </c>
-      <c r="B60" t="n">
+      <c r="B60">
         <v>1</v>
       </c>
       <c r="C60" t="s">
@@ -2009,11 +2023,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="61">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
         <v>8</v>
       </c>
-      <c r="B61" t="n">
+      <c r="B61">
         <v>0</v>
       </c>
       <c r="C61" t="s">
@@ -2035,11 +2049,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="62">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
         <v>28</v>
       </c>
-      <c r="B62" t="n">
+      <c r="B62">
         <v>0</v>
       </c>
       <c r="C62" t="s">
@@ -2061,11 +2075,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="63">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
         <v>8</v>
       </c>
-      <c r="B63" t="n">
+      <c r="B63">
         <v>1</v>
       </c>
       <c r="C63" t="s">
@@ -2087,11 +2101,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="64">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
         <v>28</v>
       </c>
-      <c r="B64" t="n">
+      <c r="B64">
         <v>1</v>
       </c>
       <c r="C64" t="s">
@@ -2113,11 +2127,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="65">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
         <v>28</v>
       </c>
-      <c r="B65" t="n">
+      <c r="B65">
         <v>0</v>
       </c>
       <c r="C65" t="s">
@@ -2139,11 +2153,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="66">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
         <v>8</v>
       </c>
-      <c r="B66" t="n">
+      <c r="B66">
         <v>1</v>
       </c>
       <c r="C66" t="s">
@@ -2165,11 +2179,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="67">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
         <v>28</v>
       </c>
-      <c r="B67" t="n">
+      <c r="B67">
         <v>1</v>
       </c>
       <c r="C67" t="s">
@@ -2191,11 +2205,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="68">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
         <v>8</v>
       </c>
-      <c r="B68" t="n">
+      <c r="B68">
         <v>1</v>
       </c>
       <c r="C68" t="s">
@@ -2217,11 +2231,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="69">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
         <v>8</v>
       </c>
-      <c r="B69" t="n">
+      <c r="B69">
         <v>1</v>
       </c>
       <c r="C69" t="s">
@@ -2243,11 +2257,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="70">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
         <v>8</v>
       </c>
-      <c r="B70" t="n">
+      <c r="B70">
         <v>0</v>
       </c>
       <c r="C70" t="s">
@@ -2269,11 +2283,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="71">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
         <v>28</v>
       </c>
-      <c r="B71" t="n">
+      <c r="B71">
         <v>0</v>
       </c>
       <c r="C71" t="s">
@@ -2295,11 +2309,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="72">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
         <v>28</v>
       </c>
-      <c r="B72" t="n">
+      <c r="B72">
         <v>0</v>
       </c>
       <c r="C72" t="s">
@@ -2321,11 +2335,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="73">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
         <v>28</v>
       </c>
-      <c r="B73" t="n">
+      <c r="B73">
         <v>0</v>
       </c>
       <c r="C73" t="s">
@@ -2347,17 +2361,16 @@
         <v>14</v>
       </c>
     </row>
-    <row r="74">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
         <v>28</v>
       </c>
-      <c r="B74" t="n">
+      <c r="B74">
         <v>0</v>
       </c>
       <c r="C74" t="s">
         <v>32</v>
       </c>
-      <c r="D74"/>
       <c r="E74" t="s">
         <v>24</v>
       </c>
@@ -2371,11 +2384,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="75">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
         <v>28</v>
       </c>
-      <c r="B75" t="n">
+      <c r="B75">
         <v>0</v>
       </c>
       <c r="C75" t="s">
@@ -2397,11 +2410,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="76">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A76" t="s">
         <v>8</v>
       </c>
-      <c r="B76" t="n">
+      <c r="B76">
         <v>1</v>
       </c>
       <c r="C76" t="s">
@@ -2423,11 +2436,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="77">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A77" t="s">
         <v>28</v>
       </c>
-      <c r="B77" t="n">
+      <c r="B77">
         <v>1</v>
       </c>
       <c r="C77" t="s">
@@ -2449,11 +2462,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="78">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A78" t="s">
         <v>28</v>
       </c>
-      <c r="B78" t="n">
+      <c r="B78">
         <v>1</v>
       </c>
       <c r="C78" t="s">
@@ -2475,11 +2488,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="79">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A79" t="s">
         <v>28</v>
       </c>
-      <c r="B79" t="n">
+      <c r="B79">
         <v>1</v>
       </c>
       <c r="C79" t="s">
@@ -2501,11 +2514,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="80">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A80" t="s">
         <v>28</v>
       </c>
-      <c r="B80" t="n">
+      <c r="B80">
         <v>0</v>
       </c>
       <c r="C80" t="s">
@@ -2527,17 +2540,16 @@
         <v>18</v>
       </c>
     </row>
-    <row r="81">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A81" t="s">
         <v>28</v>
       </c>
-      <c r="B81" t="n">
+      <c r="B81">
         <v>0</v>
       </c>
       <c r="C81" t="s">
         <v>15</v>
       </c>
-      <c r="D81"/>
       <c r="E81" t="s">
         <v>21</v>
       </c>
@@ -2551,11 +2563,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="82">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A82" t="s">
         <v>28</v>
       </c>
-      <c r="B82" t="n">
+      <c r="B82">
         <v>0</v>
       </c>
       <c r="C82" t="s">
@@ -2577,11 +2589,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="83">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A83" t="s">
         <v>28</v>
       </c>
-      <c r="B83" t="n">
+      <c r="B83">
         <v>0</v>
       </c>
       <c r="C83" t="s">
@@ -2603,11 +2615,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="84">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A84" t="s">
         <v>28</v>
       </c>
-      <c r="B84" t="n">
+      <c r="B84">
         <v>0</v>
       </c>
       <c r="C84" t="s">
@@ -2629,11 +2641,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="85">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A85" t="s">
         <v>8</v>
       </c>
-      <c r="B85" t="n">
+      <c r="B85">
         <v>0</v>
       </c>
       <c r="C85" t="s">
@@ -2655,11 +2667,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="86">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A86" t="s">
         <v>28</v>
       </c>
-      <c r="B86" t="n">
+      <c r="B86">
         <v>0</v>
       </c>
       <c r="C86" t="s">
@@ -2681,11 +2693,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="87">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A87" t="s">
         <v>8</v>
       </c>
-      <c r="B87" t="n">
+      <c r="B87">
         <v>1</v>
       </c>
       <c r="C87" t="s">
@@ -2707,11 +2719,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="88">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A88" t="s">
         <v>28</v>
       </c>
-      <c r="B88" t="n">
+      <c r="B88">
         <v>1</v>
       </c>
       <c r="C88" t="s">
@@ -2733,11 +2745,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="89">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A89" t="s">
         <v>28</v>
       </c>
-      <c r="B89" t="n">
+      <c r="B89">
         <v>1</v>
       </c>
       <c r="C89" t="s">
@@ -2759,17 +2771,16 @@
         <v>18</v>
       </c>
     </row>
-    <row r="90">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A90" t="s">
         <v>8</v>
       </c>
-      <c r="B90" t="n">
+      <c r="B90">
         <v>1</v>
       </c>
       <c r="C90" t="s">
         <v>15</v>
       </c>
-      <c r="D90"/>
       <c r="E90" t="s">
         <v>36</v>
       </c>
@@ -2783,11 +2794,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="91">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A91" t="s">
         <v>28</v>
       </c>
-      <c r="B91" t="n">
+      <c r="B91">
         <v>0</v>
       </c>
       <c r="C91" t="s">
@@ -2809,11 +2820,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="92">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A92" t="s">
         <v>8</v>
       </c>
-      <c r="B92" t="n">
+      <c r="B92">
         <v>1</v>
       </c>
       <c r="C92" t="s">
@@ -2835,11 +2846,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="93">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A93" t="s">
         <v>8</v>
       </c>
-      <c r="B93" t="n">
+      <c r="B93">
         <v>0</v>
       </c>
       <c r="C93" t="s">
@@ -2861,11 +2872,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="94">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A94" t="s">
         <v>28</v>
       </c>
-      <c r="B94" t="n">
+      <c r="B94">
         <v>0</v>
       </c>
       <c r="C94" t="s">
@@ -2887,11 +2898,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="95">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A95" t="s">
         <v>28</v>
       </c>
-      <c r="B95" t="n">
+      <c r="B95">
         <v>0</v>
       </c>
       <c r="C95" t="s">
@@ -2913,11 +2924,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="96">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A96" t="s">
         <v>28</v>
       </c>
-      <c r="B96" t="n">
+      <c r="B96">
         <v>1</v>
       </c>
       <c r="C96" t="s">
@@ -2939,11 +2950,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="97">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A97" t="s">
         <v>8</v>
       </c>
-      <c r="B97" t="n">
+      <c r="B97">
         <v>0</v>
       </c>
       <c r="C97" t="s">
@@ -2965,11 +2976,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="98">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A98" t="s">
         <v>8</v>
       </c>
-      <c r="B98" t="n">
+      <c r="B98">
         <v>1</v>
       </c>
       <c r="C98" t="s">
@@ -2991,11 +3002,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="99">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A99" t="s">
         <v>8</v>
       </c>
-      <c r="B99" t="n">
+      <c r="B99">
         <v>1</v>
       </c>
       <c r="C99" t="s">
@@ -3017,17 +3028,16 @@
         <v>18</v>
       </c>
     </row>
-    <row r="100">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A100" t="s">
         <v>8</v>
       </c>
-      <c r="B100" t="n">
+      <c r="B100">
         <v>0</v>
       </c>
       <c r="C100" t="s">
         <v>30</v>
       </c>
-      <c r="D100"/>
       <c r="E100" t="s">
         <v>22</v>
       </c>
@@ -3041,11 +3051,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="101">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A101" t="s">
         <v>8</v>
       </c>
-      <c r="B101" t="n">
+      <c r="B101">
         <v>1</v>
       </c>
       <c r="C101" t="s">
@@ -3067,11 +3077,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="102">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A102" t="s">
         <v>28</v>
       </c>
-      <c r="B102" t="n">
+      <c r="B102">
         <v>1</v>
       </c>
       <c r="C102" t="s">
@@ -3093,11 +3103,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="103">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A103" t="s">
         <v>8</v>
       </c>
-      <c r="B103" t="n">
+      <c r="B103">
         <v>0</v>
       </c>
       <c r="C103" t="s">
@@ -3119,11 +3129,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="104">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A104" t="s">
         <v>28</v>
       </c>
-      <c r="B104" t="n">
+      <c r="B104">
         <v>0</v>
       </c>
       <c r="C104" t="s">
@@ -3145,11 +3155,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="105">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A105" t="s">
         <v>8</v>
       </c>
-      <c r="B105" t="n">
+      <c r="B105">
         <v>0</v>
       </c>
       <c r="C105" t="s">
@@ -3171,11 +3181,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="106">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A106" t="s">
         <v>28</v>
       </c>
-      <c r="B106" t="n">
+      <c r="B106">
         <v>1</v>
       </c>
       <c r="C106" t="s">
@@ -3197,11 +3207,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="107">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A107" t="s">
         <v>8</v>
       </c>
-      <c r="B107" t="n">
+      <c r="B107">
         <v>1</v>
       </c>
       <c r="C107" t="s">
@@ -3223,11 +3233,11 @@
         <v>37</v>
       </c>
     </row>
-    <row r="108">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A108" t="s">
         <v>8</v>
       </c>
-      <c r="B108" t="n">
+      <c r="B108">
         <v>1</v>
       </c>
       <c r="C108" t="s">
@@ -3249,11 +3259,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="109">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A109" t="s">
         <v>28</v>
       </c>
-      <c r="B109" t="n">
+      <c r="B109">
         <v>1</v>
       </c>
       <c r="C109" t="s">
@@ -3275,11 +3285,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="110">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A110" t="s">
         <v>28</v>
       </c>
-      <c r="B110" t="n">
+      <c r="B110">
         <v>0</v>
       </c>
       <c r="C110" t="s">
@@ -3301,11 +3311,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="111">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A111" t="s">
         <v>28</v>
       </c>
-      <c r="B111" t="n">
+      <c r="B111">
         <v>0</v>
       </c>
       <c r="C111" t="s">
@@ -3327,11 +3337,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="112">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A112" t="s">
         <v>8</v>
       </c>
-      <c r="B112" t="n">
+      <c r="B112">
         <v>0</v>
       </c>
       <c r="C112" t="s">
@@ -3353,11 +3363,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="113">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A113" t="s">
         <v>8</v>
       </c>
-      <c r="B113" t="n">
+      <c r="B113">
         <v>1</v>
       </c>
       <c r="C113" t="s">
@@ -3379,11 +3389,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="114">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A114" t="s">
         <v>28</v>
       </c>
-      <c r="B114" t="n">
+      <c r="B114">
         <v>0</v>
       </c>
       <c r="C114" t="s">
@@ -3405,11 +3415,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="115">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A115" t="s">
         <v>28</v>
       </c>
-      <c r="B115" t="n">
+      <c r="B115">
         <v>0</v>
       </c>
       <c r="C115" t="s">
@@ -3431,11 +3441,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="116">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A116" t="s">
         <v>8</v>
       </c>
-      <c r="B116" t="n">
+      <c r="B116">
         <v>1</v>
       </c>
       <c r="C116" t="s">
@@ -3457,11 +3467,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="117">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A117" t="s">
         <v>8</v>
       </c>
-      <c r="B117" t="n">
+      <c r="B117">
         <v>0</v>
       </c>
       <c r="C117" t="s">
@@ -3483,11 +3493,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="118">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A118" t="s">
         <v>28</v>
       </c>
-      <c r="B118" t="n">
+      <c r="B118">
         <v>0</v>
       </c>
       <c r="C118" t="s">
@@ -3509,11 +3519,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="119">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A119" t="s">
         <v>28</v>
       </c>
-      <c r="B119" t="n">
+      <c r="B119">
         <v>1</v>
       </c>
       <c r="C119" t="s">
@@ -3535,11 +3545,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="120">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A120" t="s">
         <v>8</v>
       </c>
-      <c r="B120" t="n">
+      <c r="B120">
         <v>0</v>
       </c>
       <c r="C120" t="s">
@@ -3561,17 +3571,16 @@
         <v>18</v>
       </c>
     </row>
-    <row r="121">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A121" t="s">
         <v>8</v>
       </c>
-      <c r="B121" t="n">
+      <c r="B121">
         <v>0</v>
       </c>
       <c r="C121" t="s">
         <v>19</v>
       </c>
-      <c r="D121"/>
       <c r="E121" t="s">
         <v>21</v>
       </c>
@@ -3585,11 +3594,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="122">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A122" t="s">
         <v>8</v>
       </c>
-      <c r="B122" t="n">
+      <c r="B122">
         <v>0</v>
       </c>
       <c r="C122" t="s">
@@ -3611,11 +3620,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="123">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A123" t="s">
         <v>8</v>
       </c>
-      <c r="B123" t="n">
+      <c r="B123">
         <v>1</v>
       </c>
       <c r="C123" t="s">
@@ -3637,11 +3646,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="124">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A124" t="s">
         <v>8</v>
       </c>
-      <c r="B124" t="n">
+      <c r="B124">
         <v>1</v>
       </c>
       <c r="C124" t="s">
@@ -3663,11 +3672,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="125">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A125" t="s">
         <v>28</v>
       </c>
-      <c r="B125" t="n">
+      <c r="B125">
         <v>0</v>
       </c>
       <c r="C125" t="s">
@@ -3689,11 +3698,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="126">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A126" t="s">
         <v>8</v>
       </c>
-      <c r="B126" t="n">
+      <c r="B126">
         <v>0</v>
       </c>
       <c r="C126" t="s">
@@ -3715,11 +3724,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="127">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A127" t="s">
         <v>8</v>
       </c>
-      <c r="B127" t="n">
+      <c r="B127">
         <v>1</v>
       </c>
       <c r="C127" t="s">
@@ -3741,11 +3750,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="128">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A128" t="s">
         <v>28</v>
       </c>
-      <c r="B128" t="n">
+      <c r="B128">
         <v>0</v>
       </c>
       <c r="C128" t="s">
@@ -3767,11 +3776,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="129">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A129" t="s">
         <v>28</v>
       </c>
-      <c r="B129" t="n">
+      <c r="B129">
         <v>1</v>
       </c>
       <c r="C129" t="s">
@@ -3793,11 +3802,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="130">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A130" t="s">
         <v>28</v>
       </c>
-      <c r="B130" t="n">
+      <c r="B130">
         <v>0</v>
       </c>
       <c r="C130" t="s">
@@ -3819,11 +3828,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="131">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A131" t="s">
         <v>28</v>
       </c>
-      <c r="B131" t="n">
+      <c r="B131">
         <v>0</v>
       </c>
       <c r="C131" t="s">
@@ -3845,11 +3854,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="132">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A132" t="s">
         <v>28</v>
       </c>
-      <c r="B132" t="n">
+      <c r="B132">
         <v>1</v>
       </c>
       <c r="C132" t="s">
@@ -3871,11 +3880,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="133">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A133" t="s">
         <v>28</v>
       </c>
-      <c r="B133" t="n">
+      <c r="B133">
         <v>0</v>
       </c>
       <c r="C133" t="s">
@@ -3897,11 +3906,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="134">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A134" t="s">
         <v>28</v>
       </c>
-      <c r="B134" t="n">
+      <c r="B134">
         <v>0</v>
       </c>
       <c r="C134" t="s">
@@ -3923,11 +3932,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="135">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A135" t="s">
         <v>8</v>
       </c>
-      <c r="B135" t="n">
+      <c r="B135">
         <v>0</v>
       </c>
       <c r="C135" t="s">
@@ -3949,11 +3958,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="136">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A136" t="s">
         <v>8</v>
       </c>
-      <c r="B136" t="n">
+      <c r="B136">
         <v>1</v>
       </c>
       <c r="C136" t="s">
@@ -3975,11 +3984,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="137">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A137" t="s">
         <v>28</v>
       </c>
-      <c r="B137" t="n">
+      <c r="B137">
         <v>0</v>
       </c>
       <c r="C137" t="s">
@@ -4001,11 +4010,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="138">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A138" t="s">
         <v>28</v>
       </c>
-      <c r="B138" t="n">
+      <c r="B138">
         <v>1</v>
       </c>
       <c r="C138" t="s">
@@ -4027,11 +4036,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="139">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A139" t="s">
         <v>28</v>
       </c>
-      <c r="B139" t="n">
+      <c r="B139">
         <v>1</v>
       </c>
       <c r="C139" t="s">
@@ -4053,11 +4062,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="140">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A140" t="s">
         <v>28</v>
       </c>
-      <c r="B140" t="n">
+      <c r="B140">
         <v>0</v>
       </c>
       <c r="C140" t="s">
@@ -4079,11 +4088,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="141">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A141" t="s">
         <v>8</v>
       </c>
-      <c r="B141" t="n">
+      <c r="B141">
         <v>0</v>
       </c>
       <c r="C141" t="s">
@@ -4105,17 +4114,16 @@
         <v>14</v>
       </c>
     </row>
-    <row r="142">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A142" t="s">
         <v>28</v>
       </c>
-      <c r="B142" t="n">
+      <c r="B142">
         <v>0</v>
       </c>
       <c r="C142" t="s">
         <v>32</v>
       </c>
-      <c r="D142"/>
       <c r="E142" t="s">
         <v>22</v>
       </c>
@@ -4129,11 +4137,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="143">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A143" t="s">
         <v>8</v>
       </c>
-      <c r="B143" t="n">
+      <c r="B143">
         <v>0</v>
       </c>
       <c r="C143" t="s">
@@ -4155,11 +4163,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="144">
+    <row r="144" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A144" t="s">
         <v>28</v>
       </c>
-      <c r="B144" t="n">
+      <c r="B144">
         <v>1</v>
       </c>
       <c r="C144" t="s">
@@ -4181,17 +4189,16 @@
         <v>14</v>
       </c>
     </row>
-    <row r="145">
+    <row r="145" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A145" t="s">
         <v>28</v>
       </c>
-      <c r="B145" t="n">
+      <c r="B145">
         <v>1</v>
       </c>
       <c r="C145" t="s">
         <v>9</v>
       </c>
-      <c r="D145"/>
       <c r="E145" t="s">
         <v>24</v>
       </c>
@@ -4205,11 +4212,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="146">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A146" t="s">
         <v>8</v>
       </c>
-      <c r="B146" t="n">
+      <c r="B146">
         <v>0</v>
       </c>
       <c r="C146" t="s">
@@ -4231,11 +4238,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="147">
+    <row r="147" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A147" t="s">
         <v>8</v>
       </c>
-      <c r="B147" t="n">
+      <c r="B147">
         <v>0</v>
       </c>
       <c r="C147" t="s">
@@ -4257,11 +4264,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="148">
+    <row r="148" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A148" t="s">
         <v>28</v>
       </c>
-      <c r="B148" t="n">
+      <c r="B148">
         <v>1</v>
       </c>
       <c r="C148" t="s">
@@ -4283,11 +4290,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="149">
+    <row r="149" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A149" t="s">
         <v>8</v>
       </c>
-      <c r="B149" t="n">
+      <c r="B149">
         <v>0</v>
       </c>
       <c r="C149" t="s">
@@ -4309,11 +4316,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="150">
+    <row r="150" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A150" t="s">
         <v>28</v>
       </c>
-      <c r="B150" t="n">
+      <c r="B150">
         <v>0</v>
       </c>
       <c r="C150" t="s">
@@ -4335,11 +4342,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="151">
+    <row r="151" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A151" t="s">
         <v>8</v>
       </c>
-      <c r="B151" t="n">
+      <c r="B151">
         <v>0</v>
       </c>
       <c r="C151" t="s">
@@ -4361,17 +4368,16 @@
         <v>14</v>
       </c>
     </row>
-    <row r="152">
+    <row r="152" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A152" t="s">
         <v>28</v>
       </c>
-      <c r="B152" t="n">
+      <c r="B152">
         <v>1</v>
       </c>
       <c r="C152" t="s">
         <v>31</v>
       </c>
-      <c r="D152"/>
       <c r="E152" t="s">
         <v>26</v>
       </c>
@@ -4385,11 +4391,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="153">
+    <row r="153" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A153" t="s">
         <v>8</v>
       </c>
-      <c r="B153" t="n">
+      <c r="B153">
         <v>1</v>
       </c>
       <c r="C153" t="s">
@@ -4411,11 +4417,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="154">
+    <row r="154" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A154" t="s">
         <v>8</v>
       </c>
-      <c r="B154" t="n">
+      <c r="B154">
         <v>0</v>
       </c>
       <c r="C154" t="s">
@@ -4437,11 +4443,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="155">
+    <row r="155" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A155" t="s">
         <v>28</v>
       </c>
-      <c r="B155" t="n">
+      <c r="B155">
         <v>1</v>
       </c>
       <c r="C155" t="s">
@@ -4463,11 +4469,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="156">
+    <row r="156" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A156" t="s">
         <v>28</v>
       </c>
-      <c r="B156" t="n">
+      <c r="B156">
         <v>1</v>
       </c>
       <c r="C156" t="s">
@@ -4489,11 +4495,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="157">
+    <row r="157" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A157" t="s">
         <v>8</v>
       </c>
-      <c r="B157" t="n">
+      <c r="B157">
         <v>0</v>
       </c>
       <c r="C157" t="s">
@@ -4515,11 +4521,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="158">
+    <row r="158" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A158" t="s">
         <v>8</v>
       </c>
-      <c r="B158" t="n">
+      <c r="B158">
         <v>1</v>
       </c>
       <c r="C158" t="s">
@@ -4541,11 +4547,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="159">
+    <row r="159" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A159" t="s">
         <v>8</v>
       </c>
-      <c r="B159" t="n">
+      <c r="B159">
         <v>0</v>
       </c>
       <c r="C159" t="s">
@@ -4567,11 +4573,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="160">
+    <row r="160" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A160" t="s">
         <v>8</v>
       </c>
-      <c r="B160" t="n">
+      <c r="B160">
         <v>0</v>
       </c>
       <c r="C160" t="s">
@@ -4593,11 +4599,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="161">
+    <row r="161" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A161" t="s">
         <v>8</v>
       </c>
-      <c r="B161" t="n">
+      <c r="B161">
         <v>0</v>
       </c>
       <c r="C161" t="s">
@@ -4619,11 +4625,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="162">
+    <row r="162" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A162" t="s">
         <v>28</v>
       </c>
-      <c r="B162" t="n">
+      <c r="B162">
         <v>1</v>
       </c>
       <c r="C162" t="s">
@@ -4645,11 +4651,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="163">
+    <row r="163" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A163" t="s">
         <v>8</v>
       </c>
-      <c r="B163" t="n">
+      <c r="B163">
         <v>0</v>
       </c>
       <c r="C163" t="s">
@@ -4671,17 +4677,16 @@
         <v>14</v>
       </c>
     </row>
-    <row r="164">
+    <row r="164" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A164" t="s">
         <v>8</v>
       </c>
-      <c r="B164" t="n">
+      <c r="B164">
         <v>0</v>
       </c>
       <c r="C164" t="s">
         <v>15</v>
       </c>
-      <c r="D164"/>
       <c r="E164" t="s">
         <v>21</v>
       </c>
@@ -4695,11 +4700,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="165">
+    <row r="165" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A165" t="s">
         <v>28</v>
       </c>
-      <c r="B165" t="n">
+      <c r="B165">
         <v>0</v>
       </c>
       <c r="C165" t="s">
@@ -4721,11 +4726,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="166">
+    <row r="166" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A166" t="s">
         <v>8</v>
       </c>
-      <c r="B166" t="n">
+      <c r="B166">
         <v>0</v>
       </c>
       <c r="C166" t="s">
@@ -4747,11 +4752,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="167">
+    <row r="167" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A167" t="s">
         <v>8</v>
       </c>
-      <c r="B167" t="n">
+      <c r="B167">
         <v>0</v>
       </c>
       <c r="C167" t="s">
@@ -4773,11 +4778,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="168">
+    <row r="168" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A168" t="s">
         <v>28</v>
       </c>
-      <c r="B168" t="n">
+      <c r="B168">
         <v>0</v>
       </c>
       <c r="C168" t="s">
@@ -4799,11 +4804,11 @@
         <v>37</v>
       </c>
     </row>
-    <row r="169">
+    <row r="169" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A169" t="s">
         <v>28</v>
       </c>
-      <c r="B169" t="n">
+      <c r="B169">
         <v>0</v>
       </c>
       <c r="C169" t="s">
@@ -4825,17 +4830,16 @@
         <v>14</v>
       </c>
     </row>
-    <row r="170">
+    <row r="170" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A170" t="s">
         <v>28</v>
       </c>
-      <c r="B170" t="n">
+      <c r="B170">
         <v>0</v>
       </c>
       <c r="C170" t="s">
         <v>19</v>
       </c>
-      <c r="D170"/>
       <c r="E170" t="s">
         <v>22</v>
       </c>
@@ -4849,11 +4853,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="171">
+    <row r="171" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A171" t="s">
         <v>8</v>
       </c>
-      <c r="B171" t="n">
+      <c r="B171">
         <v>0</v>
       </c>
       <c r="C171" t="s">
@@ -4875,11 +4879,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="172">
+    <row r="172" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A172" t="s">
         <v>8</v>
       </c>
-      <c r="B172" t="n">
+      <c r="B172">
         <v>1</v>
       </c>
       <c r="C172" t="s">
@@ -4901,11 +4905,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="173">
+    <row r="173" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A173" t="s">
         <v>28</v>
       </c>
-      <c r="B173" t="n">
+      <c r="B173">
         <v>0</v>
       </c>
       <c r="C173" t="s">
@@ -4927,11 +4931,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="174">
+    <row r="174" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A174" t="s">
         <v>8</v>
       </c>
-      <c r="B174" t="n">
+      <c r="B174">
         <v>1</v>
       </c>
       <c r="C174" t="s">
@@ -4953,11 +4957,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="175">
+    <row r="175" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A175" t="s">
         <v>28</v>
       </c>
-      <c r="B175" t="n">
+      <c r="B175">
         <v>0</v>
       </c>
       <c r="C175" t="s">
@@ -4979,17 +4983,16 @@
         <v>14</v>
       </c>
     </row>
-    <row r="176">
+    <row r="176" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A176" t="s">
         <v>28</v>
       </c>
-      <c r="B176" t="n">
+      <c r="B176">
         <v>0</v>
       </c>
       <c r="C176" t="s">
         <v>32</v>
       </c>
-      <c r="D176"/>
       <c r="E176" t="s">
         <v>22</v>
       </c>
@@ -5003,11 +5006,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="177">
+    <row r="177" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A177" t="s">
         <v>28</v>
       </c>
-      <c r="B177" t="n">
+      <c r="B177">
         <v>0</v>
       </c>
       <c r="C177" t="s">
@@ -5029,11 +5032,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="178">
+    <row r="178" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A178" t="s">
         <v>8</v>
       </c>
-      <c r="B178" t="n">
+      <c r="B178">
         <v>1</v>
       </c>
       <c r="C178" t="s">
@@ -5055,11 +5058,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="179">
+    <row r="179" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A179" t="s">
         <v>28</v>
       </c>
-      <c r="B179" t="n">
+      <c r="B179">
         <v>1</v>
       </c>
       <c r="C179" t="s">
@@ -5081,11 +5084,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="180">
+    <row r="180" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A180" t="s">
         <v>8</v>
       </c>
-      <c r="B180" t="n">
+      <c r="B180">
         <v>0</v>
       </c>
       <c r="C180" t="s">
@@ -5107,11 +5110,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="181">
+    <row r="181" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A181" t="s">
         <v>8</v>
       </c>
-      <c r="B181" t="n">
+      <c r="B181">
         <v>1</v>
       </c>
       <c r="C181" t="s">
@@ -5133,11 +5136,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="182">
+    <row r="182" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A182" t="s">
         <v>28</v>
       </c>
-      <c r="B182" t="n">
+      <c r="B182">
         <v>1</v>
       </c>
       <c r="C182" t="s">
@@ -5159,11 +5162,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="183">
+    <row r="183" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A183" t="s">
         <v>28</v>
       </c>
-      <c r="B183" t="n">
+      <c r="B183">
         <v>0</v>
       </c>
       <c r="C183" t="s">
@@ -5185,11 +5188,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="184">
+    <row r="184" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A184" t="s">
         <v>28</v>
       </c>
-      <c r="B184" t="n">
+      <c r="B184">
         <v>1</v>
       </c>
       <c r="C184" t="s">
@@ -5211,11 +5214,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="185">
+    <row r="185" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A185" t="s">
         <v>8</v>
       </c>
-      <c r="B185" t="n">
+      <c r="B185">
         <v>0</v>
       </c>
       <c r="C185" t="s">
@@ -5237,11 +5240,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="186">
+    <row r="186" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A186" t="s">
         <v>8</v>
       </c>
-      <c r="B186" t="n">
+      <c r="B186">
         <v>1</v>
       </c>
       <c r="C186" t="s">
@@ -5263,11 +5266,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="187">
+    <row r="187" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A187" t="s">
         <v>8</v>
       </c>
-      <c r="B187" t="n">
+      <c r="B187">
         <v>0</v>
       </c>
       <c r="C187" t="s">
@@ -5289,11 +5292,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="188">
+    <row r="188" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A188" t="s">
         <v>28</v>
       </c>
-      <c r="B188" t="n">
+      <c r="B188">
         <v>0</v>
       </c>
       <c r="C188" t="s">
@@ -5315,11 +5318,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="189">
+    <row r="189" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A189" t="s">
         <v>8</v>
       </c>
-      <c r="B189" t="n">
+      <c r="B189">
         <v>0</v>
       </c>
       <c r="C189" t="s">
@@ -5341,11 +5344,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="190">
+    <row r="190" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A190" t="s">
         <v>28</v>
       </c>
-      <c r="B190" t="n">
+      <c r="B190">
         <v>1</v>
       </c>
       <c r="C190" t="s">
@@ -5367,11 +5370,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="191">
+    <row r="191" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A191" t="s">
         <v>28</v>
       </c>
-      <c r="B191" t="n">
+      <c r="B191">
         <v>1</v>
       </c>
       <c r="C191" t="s">
@@ -5393,11 +5396,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="192">
+    <row r="192" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A192" t="s">
         <v>8</v>
       </c>
-      <c r="B192" t="n">
+      <c r="B192">
         <v>1</v>
       </c>
       <c r="C192" t="s">
@@ -5419,11 +5422,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="193">
+    <row r="193" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A193" t="s">
         <v>28</v>
       </c>
-      <c r="B193" t="n">
+      <c r="B193">
         <v>0</v>
       </c>
       <c r="C193" t="s">
@@ -5445,17 +5448,16 @@
         <v>18</v>
       </c>
     </row>
-    <row r="194">
+    <row r="194" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A194" t="s">
         <v>8</v>
       </c>
-      <c r="B194" t="n">
+      <c r="B194">
         <v>1</v>
       </c>
       <c r="C194" t="s">
         <v>32</v>
       </c>
-      <c r="D194"/>
       <c r="E194" t="s">
         <v>21</v>
       </c>
@@ -5469,17 +5471,16 @@
         <v>18</v>
       </c>
     </row>
-    <row r="195">
+    <row r="195" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A195" t="s">
         <v>8</v>
       </c>
-      <c r="B195" t="n">
+      <c r="B195">
         <v>0</v>
       </c>
       <c r="C195" t="s">
         <v>23</v>
       </c>
-      <c r="D195"/>
       <c r="E195" t="s">
         <v>21</v>
       </c>
@@ -5493,11 +5494,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="196">
+    <row r="196" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A196" t="s">
         <v>28</v>
       </c>
-      <c r="B196" t="n">
+      <c r="B196">
         <v>0</v>
       </c>
       <c r="C196" t="s">
@@ -5519,11 +5520,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="197">
+    <row r="197" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A197" t="s">
         <v>8</v>
       </c>
-      <c r="B197" t="n">
+      <c r="B197">
         <v>1</v>
       </c>
       <c r="C197" t="s">
@@ -5545,11 +5546,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="198">
+    <row r="198" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A198" t="s">
         <v>8</v>
       </c>
-      <c r="B198" t="n">
+      <c r="B198">
         <v>0</v>
       </c>
       <c r="C198" t="s">
@@ -5571,11 +5572,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="199">
+    <row r="199" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A199" t="s">
         <v>28</v>
       </c>
-      <c r="B199" t="n">
+      <c r="B199">
         <v>1</v>
       </c>
       <c r="C199" t="s">
@@ -5597,11 +5598,11 @@
         <v>37</v>
       </c>
     </row>
-    <row r="200">
+    <row r="200" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A200" t="s">
         <v>28</v>
       </c>
-      <c r="B200" t="n">
+      <c r="B200">
         <v>1</v>
       </c>
       <c r="C200" t="s">
@@ -5623,11 +5624,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="201">
+    <row r="201" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A201" t="s">
         <v>28</v>
       </c>
-      <c r="B201" t="n">
+      <c r="B201">
         <v>0</v>
       </c>
       <c r="C201" t="s">
@@ -5651,6 +5652,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>